<commit_message>
aggiunta metodo a monte
</commit_message>
<xml_diff>
--- a/esperimento_1/esperimento1.xlsx
+++ b/esperimento_1/esperimento1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pierl\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1796579-5942-4531-9C16-FBD35175DA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DE7B90-8D4E-47C3-A46D-D9E7D3B0C7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1D46AA1E-C215-4195-901F-99D92B2A9D67}"/>
   </bookViews>
@@ -411,15 +411,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A04E809-241E-4C3A-A23F-46CB2C91F703}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>-20</v>
       </c>
@@ -448,8 +448,17 @@
       <c r="K1">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M1">
+        <v>-20</v>
+      </c>
+      <c r="N1">
+        <v>-19.98</v>
+      </c>
+      <c r="O1">
+        <v>-34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>-16</v>
       </c>
@@ -478,8 +487,17 @@
       <c r="K2">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M2">
+        <v>-16</v>
+      </c>
+      <c r="N2">
+        <v>-15.95</v>
+      </c>
+      <c r="O2">
+        <v>-27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>-12</v>
       </c>
@@ -508,8 +526,17 @@
       <c r="K3">
         <v>200</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M3">
+        <v>-12</v>
+      </c>
+      <c r="N3">
+        <v>-11.99</v>
+      </c>
+      <c r="O3">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>-8</v>
       </c>
@@ -538,8 +565,18 @@
       <c r="K4">
         <v>390</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M4">
+        <v>-8</v>
+      </c>
+      <c r="N4">
+        <v>-8.0299999999999994</v>
+      </c>
+      <c r="O4">
+        <v>-14</v>
+      </c>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>-4</v>
       </c>
@@ -568,8 +605,17 @@
       <c r="K5">
         <v>15000</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M5">
+        <v>-4</v>
+      </c>
+      <c r="N5">
+        <v>-3.97</v>
+      </c>
+      <c r="O5">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
@@ -588,8 +634,17 @@
       <c r="G6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
@@ -609,8 +664,17 @@
       <c r="G7">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M7">
+        <v>4</v>
+      </c>
+      <c r="N7">
+        <v>4</v>
+      </c>
+      <c r="O7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -629,8 +693,17 @@
       <c r="G8">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M8">
+        <v>8</v>
+      </c>
+      <c r="N8">
+        <v>8.01</v>
+      </c>
+      <c r="O8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>12</v>
       </c>
@@ -649,8 +722,17 @@
       <c r="G9">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M9">
+        <v>12</v>
+      </c>
+      <c r="N9">
+        <v>12.03</v>
+      </c>
+      <c r="O9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>16</v>
       </c>
@@ -669,8 +751,17 @@
       <c r="G10">
         <v>70</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M10">
+        <v>16</v>
+      </c>
+      <c r="N10">
+        <v>15.95</v>
+      </c>
+      <c r="O10">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>20</v>
       </c>
@@ -688,6 +779,15 @@
       </c>
       <c r="G11">
         <v>80</v>
+      </c>
+      <c r="M11">
+        <v>20</v>
+      </c>
+      <c r="N11">
+        <v>19.96</v>
+      </c>
+      <c r="O11">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>